<commit_message>
Revise and complete draft analysis of frequencies
</commit_message>
<xml_diff>
--- a/Extension Category.xlsx
+++ b/Extension Category.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="Extension_Category"/>
   </sheets>
   <definedNames>
-    <definedName name="Extension_Category">'Extension_Category'!$A$1:$D$12</definedName>
+    <definedName name="Extension_Category">'Extension_Category'!$A$1:$D$13</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -343,7 +343,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -384,7 +384,7 @@
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>Track trasport of pollutants, particles, or objects</t>
+          <t>Track transport of pollutants, particles, or objects</t>
         </is>
       </c>
       <c r="D2" s="0">
@@ -397,7 +397,7 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Water Quality Model</t>
+          <t>Acidification Model</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
@@ -406,7 +406,7 @@
         </is>
       </c>
       <c r="D3" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="4">
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="D6" s="0">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row outlineLevel="0" r="7">
@@ -474,7 +474,7 @@
       </c>
       <c r="C7" s="0" t="inlineStr">
         <is>
-          <t>Predicts flooding or innundation</t>
+          <t>Predicts flooding or inundation</t>
         </is>
       </c>
       <c r="D7" s="0">
@@ -483,70 +483,70 @@
     </row>
     <row outlineLevel="0" r="8">
       <c r="A8" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>Stormwater or Drainage Model</t>
+          <t>Watershed Model</t>
         </is>
       </c>
       <c r="C8" s="0" t="inlineStr">
         <is>
-          <t>Estimate water yield and pollutant loads from uplands or drainage system</t>
+          <t>Watershed model or urban drainage model of water flow and nutrient loads</t>
         </is>
       </c>
       <c r="D8" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row outlineLevel="0" r="9">
       <c r="A9" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>River Discharge Model</t>
+          <t>Ecosystem Model</t>
         </is>
       </c>
       <c r="C9" s="0" t="inlineStr">
         <is>
-          <t>Estimate river discharge</t>
+          <t>Predict ecosystem response to conditions and nutrient loading</t>
         </is>
       </c>
       <c r="D9" s="0">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="10">
       <c r="A10" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>Watershed Model</t>
+          <t>Ice models</t>
         </is>
       </c>
       <c r="C10" s="0" t="inlineStr">
         <is>
-          <t>Watershed model of water and nutrient loads</t>
+          <t>Models that predict freezing of the harbor, ice damage, or icing of ship and boat superstructure</t>
         </is>
       </c>
       <c r="D10" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row outlineLevel="0" r="11">
       <c r="A11" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>Not Specified</t>
+          <t>Habitat Models</t>
         </is>
       </c>
       <c r="C11" s="0" t="inlineStr">
         <is>
-          <t>No specific model extension implied</t>
+          <t>Models that predict habitat conditions or suitability</t>
         </is>
       </c>
       <c r="D11" s="0">
@@ -555,20 +555,38 @@
     </row>
     <row outlineLevel="0" r="12">
       <c r="A12" s="0">
+        <v>17</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>Use Capabilities</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>Extensions that allow application of the model in different ways or settings</t>
+        </is>
+      </c>
+      <c r="D12" s="0">
         <v>12</v>
       </c>
-      <c r="B12" s="0" t="inlineStr">
-        <is>
-          <t>Ecosystem Model</t>
-        </is>
-      </c>
-      <c r="C12" s="0" t="inlineStr">
-        <is>
-          <t>Predict ecosystem response to conditions and nutirent loading</t>
-        </is>
-      </c>
-      <c r="D12" s="0">
-        <v>2</v>
+    </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="0">
+        <v>18</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>Model Refinement</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>Improvements in resolution or accuracy of the model to address specific needs</t>
+        </is>
+      </c>
+      <c r="D13" s="0">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>